<commit_message>
Placed some code in comments
</commit_message>
<xml_diff>
--- a/STEP4/PlasForest_Summary.xlsx
+++ b/STEP4/PlasForest_Summary.xlsx
@@ -1866,11 +1866,11 @@
   </sheetPr>
   <dimension ref="A1:G358"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A304" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A155" activeCellId="0" sqref="A155"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.71"/>
@@ -2927,11 +2927,11 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="6"/>
-      <c r="B103" s="6" t="s">
+      <c r="A103" s="12"/>
+      <c r="B103" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="C103" s="7" t="s">
+      <c r="C103" s="13" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>